<commit_message>
Upload the traditional matrix multiplication.
</commit_message>
<xml_diff>
--- a/Mini Project 1/Test_Result.xlsx
+++ b/Mini Project 1/Test_Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eeb1337d597c500e/Documents/Rensselaer Polytechnic Institute/ECSE4961/Assignments/1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_F25DC773A252ABDACC1048F0391A74DE5BDE58EA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7FB29314-FF67-43F2-9FD1-CE3A19EEB0A6}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="11_F25DC773A252ABDACC1048F0391A74DE5BDE58EA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{796CEB15-C14D-4956-8844-5390E81F0CA3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Results</c:v>
+                  <c:v>Float Results</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Traditional</c:v>
@@ -303,34 +303,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.92200000000000004</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.274</c:v>
+                  <c:v>4.8360000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.497</c:v>
+                  <c:v>16.401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.412999999999997</c:v>
+                  <c:v>38.927999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>111.705</c:v>
+                  <c:v>76.033000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>192.93</c:v>
+                  <c:v>131.85900000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>305.39100000000002</c:v>
+                  <c:v>208.809</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>457.29199999999997</c:v>
+                  <c:v>312.774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>649.27499999999998</c:v>
+                  <c:v>443.23700000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>870.35799999999995</c:v>
+                  <c:v>609.21199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -350,7 +350,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Results</c:v>
+                  <c:v>Float Results</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Optimized</c:v>
@@ -647,7 +647,544 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Int</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Results</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Results</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Traditional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>int 1000*1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>int 2000*2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int 3000*3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>int 4000*4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>int 5000*5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>int 6000*6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>int 7000*7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>int 8000*8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>int 9000*9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>int 10000*10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.58199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9720000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.312999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.896999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73.917000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.797</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>202.16900000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>303.73099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>436.89699999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>595.43100000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-47A5-4613-8BA7-2A9F0F316E5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Results</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Optimized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Results!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>int 1000*1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>int 2000*2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>int 3000*3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>int 4000*4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>int 5000*5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>int 6000*6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>int 7000*7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>int 8000*8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>int 9000*9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>int 10000*10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-47A5-4613-8BA7-2A9F0F316E5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="987328191"/>
+        <c:axId val="987327775"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="987328191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987327775"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="987327775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987328191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1190,6 +1727,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1223,6 +2263,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DC7F4B7-F61E-45E1-B9A9-F283C1D21320}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1497,7 +2573,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +2603,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1538,7 +2614,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4.9720000000000004</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1549,7 +2625,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>16.312999999999999</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1560,7 +2636,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>37.896999999999998</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1571,7 +2647,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>73.917000000000002</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1582,7 +2658,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>127.797</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1593,7 +2669,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>202.16900000000001</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1604,7 +2680,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>303.73099999999999</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1615,7 +2691,7 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>436.89699999999999</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1626,7 +2702,7 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>595.43100000000004</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1652,7 +2728,7 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>0.92200000000000004</v>
+        <v>0.61</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1663,7 +2739,7 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>7.274</v>
+        <v>4.8360000000000003</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1674,7 +2750,7 @@
         <v>9</v>
       </c>
       <c r="B26">
-        <v>24.497</v>
+        <v>16.401</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1685,7 +2761,7 @@
         <v>10</v>
       </c>
       <c r="B27">
-        <v>57.412999999999997</v>
+        <v>38.927999999999997</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1696,7 +2772,7 @@
         <v>6</v>
       </c>
       <c r="B28">
-        <v>111.705</v>
+        <v>76.033000000000001</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1707,7 +2783,7 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>192.93</v>
+        <v>131.85900000000001</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1718,7 +2794,7 @@
         <v>13</v>
       </c>
       <c r="B30">
-        <v>305.39100000000002</v>
+        <v>208.809</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1729,7 +2805,7 @@
         <v>11</v>
       </c>
       <c r="B31">
-        <v>457.29199999999997</v>
+        <v>312.774</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1740,7 +2816,7 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <v>649.27499999999998</v>
+        <v>443.23700000000002</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1751,7 +2827,7 @@
         <v>5</v>
       </c>
       <c r="B33">
-        <v>870.35799999999995</v>
+        <v>609.21199999999999</v>
       </c>
       <c r="C33">
         <v>0</v>

</xml_diff>